<commit_message>
Onsite bug fixing for hardware
</commit_message>
<xml_diff>
--- a/.config/becExpConfig/becExpType.csv.xlsx
+++ b/.config/becExpConfig/becExpType.csv.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="966">
   <si>
     <t>TrialName</t>
   </si>
@@ -2862,6 +2862,72 @@
   </si>
   <si>
     <t>SineFit1D</t>
+  </si>
+  <si>
+    <t>MotIMCDetuning</t>
+  </si>
+  <si>
+    <t>A TOF experiment after MOT stage.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>IMCDetuning</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>RandomPolarization</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>MotIMCDetuning</t>
+  </si>
+  <si>
+    <t>An experiment after MOT stage. Scan IMC detuning.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>IMCDetuning</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>RandomPolarization</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
   </si>
 </sst>
 </file>
@@ -3188,7 +3254,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O62"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView tabSelected="true" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
@@ -6037,6 +6103,51 @@
         <v>931</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" s="0" t="s">
+        <v>955</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>956</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>957</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>958</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>959</v>
+      </c>
+      <c r="F63" s="0">
+        <v>4</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>960</v>
+      </c>
+      <c r="H63" s="0"/>
+      <c r="I63" s="0" t="s">
+        <v>961</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>962</v>
+      </c>
+      <c r="K63" s="0" t="s">
+        <v>963</v>
+      </c>
+      <c r="L63" s="0">
+        <v>8</v>
+      </c>
+      <c r="M63" s="0" t="s">
+        <v>964</v>
+      </c>
+      <c r="N63" s="0">
+        <v>30</v>
+      </c>
+      <c r="O63" s="0" t="s">
+        <v>965</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed amplitude bugs in setting keysight ARB files
</commit_message>
<xml_diff>
--- a/.config/becExpConfig/becExpType.csv.xlsx
+++ b/.config/becExpConfig/becExpType.csv.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="1014">
   <si>
     <t>TrialName</t>
   </si>
@@ -2928,6 +2928,150 @@
   </si>
   <si>
     <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>partialEvapDpartialevaptime</t>
+  </si>
+  <si>
+    <t>An experiment at partial evaporation stage D.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>EvapDOdt1</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>partialevaptime</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>RandomPolarization</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>HfBecCurveField</t>
+  </si>
+  <si>
+    <t>An experiment at the high-field BEC stage.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>curveField</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>StrongLight</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>HfBecCurveField</t>
+  </si>
+  <si>
+    <t>An experiment at the high-field BEC stage. Scan curveField.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>Bec</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>curveField</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>StrongLight</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>LinearFit1D</t>
+  </si>
+  <si>
+    <t>NiBecCameraOdt</t>
+  </si>
+  <si>
+    <t>An experiment at the non-interacting BEC stage. Use the ODT camera</t>
+  </si>
+  <si>
+    <t>ODT</t>
+  </si>
+  <si>
+    <t>SideOdtCamera</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>RunIndex</t>
+  </si>
+  <si>
+    <t>DensityFit;AtomNumber;CenterFit</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>TwoLevelWeakLight</t>
+  </si>
+  <si>
+    <t>BosonicGaussianFit1D</t>
+  </si>
+  <si>
+    <t>ParabolicFit1D</t>
   </si>
 </sst>
 </file>
@@ -3254,7 +3398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView tabSelected="true" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
@@ -3262,7 +3406,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="true"/>
+    <col min="1" max="1" width="26.42578125" customWidth="true"/>
     <col min="2" max="2" width="95.28515625" customWidth="true"/>
     <col min="3" max="3" width="16.42578125" customWidth="true"/>
     <col min="4" max="4" width="18.85546875" customWidth="true"/>
@@ -5402,50 +5546,50 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s">
-        <v>489</v>
-      </c>
-      <c r="B48" t="s">
-        <v>490</v>
-      </c>
-      <c r="C48" t="s">
-        <v>491</v>
-      </c>
-      <c r="D48" t="s">
-        <v>492</v>
-      </c>
-      <c r="E48" t="s">
-        <v>493</v>
-      </c>
-      <c r="F48">
-        <v>4</v>
-      </c>
-      <c r="G48" t="s">
-        <v>494</v>
-      </c>
-      <c r="H48" t="s">
-        <v>495</v>
-      </c>
-      <c r="I48" t="s">
-        <v>496</v>
-      </c>
-      <c r="J48" t="s">
-        <v>497</v>
-      </c>
-      <c r="K48" t="s">
-        <v>498</v>
-      </c>
-      <c r="L48">
-        <v>8</v>
-      </c>
-      <c r="M48" t="s">
-        <v>499</v>
-      </c>
-      <c r="N48">
-        <v>0.2</v>
-      </c>
-      <c r="O48" t="s">
-        <v>500</v>
+      <c r="A48" s="0" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F48" s="0">
+        <v>4</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>1007</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>1008</v>
+      </c>
+      <c r="I48" s="0" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>1010</v>
+      </c>
+      <c r="K48" s="0" t="s">
+        <v>1011</v>
+      </c>
+      <c r="L48" s="0">
+        <v>4</v>
+      </c>
+      <c r="M48" s="0" t="s">
+        <v>1012</v>
+      </c>
+      <c r="N48" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="O48" s="0" t="s">
+        <v>1013</v>
       </c>
     </row>
     <row r="49">
@@ -6146,6 +6290,100 @@
       </c>
       <c r="O63" s="0" t="s">
         <v>965</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="s">
+        <v>966</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>967</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>968</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>969</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>970</v>
+      </c>
+      <c r="F64" s="0">
+        <v>4</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>971</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>972</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>973</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>974</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>975</v>
+      </c>
+      <c r="L64" s="0">
+        <v>8</v>
+      </c>
+      <c r="M64" s="0" t="s">
+        <v>976</v>
+      </c>
+      <c r="N64" s="0">
+        <v>30</v>
+      </c>
+      <c r="O64" s="0" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="s">
+        <v>990</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>991</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>992</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>993</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>994</v>
+      </c>
+      <c r="F65" s="0">
+        <v>4</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>995</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>996</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>997</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>998</v>
+      </c>
+      <c r="K65" s="0" t="s">
+        <v>999</v>
+      </c>
+      <c r="L65" s="0">
+        <v>8</v>
+      </c>
+      <c r="M65" s="0" t="s">
+        <v>1000</v>
+      </c>
+      <c r="N65" s="0">
+        <v>2</v>
+      </c>
+      <c r="O65" s="0" t="s">
+        <v>1001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>